<commit_message>
SignIn function has been added
</commit_message>
<xml_diff>
--- a/MarsAdvancedTask/DataFiles/LoginData.xlsx
+++ b/MarsAdvancedTask/DataFiles/LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="17780"/>
+    <workbookView windowWidth="19420" windowHeight="17180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationData" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -38,7 +38,7 @@
     <t>He</t>
   </si>
   <si>
-    <t>eddie309@gmail.com</t>
+    <t>eddie510@gmail.com</t>
   </si>
   <si>
     <t>eddie123</t>
@@ -65,25 +65,22 @@
     <t>eddie789</t>
   </si>
   <si>
+    <t>eddie123@gmail.com</t>
+  </si>
+  <si>
+    <t>!@#@!</t>
+  </si>
+  <si>
+    <t>!#!#!@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>!@#!#@</t>
+  </si>
+  <si>
     <t>eddie123@gamil.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>!@#@!</t>
-  </si>
-  <si>
-    <t>!#!#!@gmail.com</t>
-  </si>
-  <si>
-    <t>!@#!#@</t>
-  </si>
-  <si>
-    <t>hlhedison112223@gamil.com</t>
-  </si>
-  <si>
-    <t>hkjhsdau1231738178ashjashdakjhgdu1</t>
   </si>
 </sst>
 </file>
@@ -96,7 +93,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +106,6 @@
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -588,48 +578,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -639,126 +632,117 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1111,8 +1095,8 @@
   <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -1126,159 +1110,159 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="16.5" spans="1:5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="7:8">
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" s="3" customFormat="1" spans="7:8">
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" s="3" customFormat="1" spans="7:8">
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,13 +1274,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="32.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="43.3636363636364" customWidth="1"/>
@@ -1311,68 +1295,52 @@
       </c>
     </row>
     <row r="2" ht="16.5" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="16.5" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" ht="16.5" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" ht="16.5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" ht="16.5" spans="1:2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" ht="16.5" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" ht="16.5" spans="1:2">
-      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>